<commit_message>
MIssing Field Data Test
</commit_message>
<xml_diff>
--- a/findbyfilewebelement/src/test/resources/excel/MultipleAccessData.xlsx
+++ b/findbyfilewebelement/src/test/resources/excel/MultipleAccessData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2190" windowWidth="15315" windowHeight="6750" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2190" windowWidth="13455" windowHeight="6750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -387,7 +387,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>